<commit_message>
Added more information and documentation
Signed-off-by: Konstruktion <racing@hochschule-stralsund.de>
</commit_message>
<xml_diff>
--- a/Schnittstellen.xlsx
+++ b/Schnittstellen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Technik\Technik 2020\04 - Electronics\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8440A2-2A3B-4410-83E7-CD0DC8702AF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B618AF-A36D-44F4-9D49-736131F7BA62}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="293">
   <si>
     <t>Gerät</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Pin Name/Notiz</t>
   </si>
   <si>
-    <t>Redcube</t>
-  </si>
-  <si>
     <t>Servo_Supply_1-3</t>
   </si>
   <si>
@@ -883,6 +880,36 @@
   </si>
   <si>
     <t>Can Extension</t>
+  </si>
+  <si>
+    <t>GND NWSU</t>
+  </si>
+  <si>
+    <t>AdapterPlatine Overall</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>60A</t>
+  </si>
+  <si>
+    <t>je 8A</t>
+  </si>
+  <si>
+    <t>15A</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
+    <t>1x10A(DCDC), 1x0.2A Signal GND</t>
+  </si>
+  <si>
+    <t>(Intern) 2.5A max</t>
+  </si>
+  <si>
+    <t>1A max.</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1085,6 +1112,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1249,8 +1277,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E31059E6-F1D6-4971-8C7E-282FD5400FF1}" name="Tabelle1" displayName="Tabelle1" ref="H2:L50" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
-  <autoFilter ref="H2:L50" xr:uid="{ACB302FC-3223-4B14-A7ED-23A1DE340AE7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E31059E6-F1D6-4971-8C7E-282FD5400FF1}" name="Tabelle1" displayName="Tabelle1" ref="H2:L51" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+  <autoFilter ref="H2:L51" xr:uid="{ACB302FC-3223-4B14-A7ED-23A1DE340AE7}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{1AB5DF06-D180-4382-A2B2-F0D8A73433A4}" name="Gerät" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{2D335D8E-C827-4BB4-AA08-16B63FE22DFB}" name="Name" dataDxfId="3"/>
@@ -1813,23 +1841,23 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="9">
         <v>2</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="9">
         <v>1</v>
@@ -1840,20 +1868,20 @@
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="9">
         <v>1</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="9">
         <v>1</v>
@@ -1864,33 +1892,33 @@
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D24" s="9">
         <v>1</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" s="9">
         <v>1</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" s="9">
         <v>1</v>
@@ -1901,7 +1929,7 @@
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" s="10">
         <v>1</v>
@@ -1911,7 +1939,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="8">
@@ -2047,19 +2075,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D773C7A0-1CF0-4EB4-B987-DAE84E5C26FF}">
-  <dimension ref="B1:X59"/>
+  <dimension ref="B1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24:L24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="11"/>
-    <col min="2" max="2" width="20" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" style="11" customWidth="1"/>
     <col min="4" max="5" width="11.42578125" style="11"/>
-    <col min="6" max="6" width="15.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="11.42578125" style="11"/>
     <col min="12" max="12" width="17.28515625" style="11" customWidth="1"/>
@@ -2072,7 +2100,7 @@
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="H1" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
@@ -2142,149 +2170,155 @@
         <v>52</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="21" t="s">
-        <v>54</v>
+        <v>286</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" s="25"/>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
       <c r="Q3" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R3" s="21"/>
       <c r="T3" s="21"/>
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
       <c r="W3" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X3" s="21"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="22"/>
       <c r="C4" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="22">
         <v>3</v>
       </c>
       <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="F4" s="22" t="s">
+        <v>285</v>
+      </c>
       <c r="G4" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L4" s="26"/>
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
       <c r="Q4" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R4" s="22"/>
       <c r="T4" s="22"/>
       <c r="U4" s="22"/>
       <c r="V4" s="22"/>
       <c r="W4" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="X4" s="22"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="21"/>
       <c r="C5" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="21">
         <v>2</v>
       </c>
       <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="F5" s="21" t="s">
+        <v>287</v>
+      </c>
       <c r="G5" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L5" s="25"/>
       <c r="N5" s="21"/>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
       <c r="Q5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R5" s="21"/>
       <c r="T5" s="21"/>
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
       <c r="W5" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="X5" s="21"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="22"/>
       <c r="C6" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+      <c r="F6" s="22" t="s">
+        <v>290</v>
+      </c>
       <c r="G6" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L6" s="26"/>
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R6" s="22"/>
       <c r="T6" s="22"/>
       <c r="U6" s="22"/>
       <c r="V6" s="22"/>
       <c r="W6" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="X6" s="22"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="21"/>
       <c r="C7" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="21">
         <v>1</v>
@@ -2292,34 +2326,34 @@
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
       <c r="G7" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L7" s="25"/>
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
       <c r="Q7" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R7" s="21"/>
       <c r="T7" s="21"/>
       <c r="U7" s="21"/>
       <c r="V7" s="21"/>
       <c r="W7" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="X7" s="21"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="22">
         <v>1</v>
@@ -2327,162 +2361,170 @@
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
       <c r="G8" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H8" s="23"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L8" s="26"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R8" s="22"/>
       <c r="T8" s="22"/>
       <c r="U8" s="22"/>
       <c r="V8" s="22"/>
       <c r="W8" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="X8" s="22"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
       <c r="C9" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="21">
         <v>1</v>
       </c>
       <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="21" t="s">
+        <v>291</v>
+      </c>
       <c r="H9" s="16"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L9" s="25"/>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R9" s="21"/>
       <c r="T9" s="21"/>
       <c r="U9" s="21"/>
       <c r="V9" s="21"/>
       <c r="W9" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="X9" s="21"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
       <c r="C10" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="22">
         <v>1</v>
       </c>
       <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
+      <c r="F10" s="22" t="s">
+        <v>288</v>
+      </c>
       <c r="H10" s="24"/>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L10" s="27"/>
       <c r="N10" s="22"/>
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R10" s="22"/>
       <c r="T10" s="22"/>
       <c r="U10" s="22"/>
       <c r="V10" s="22"/>
       <c r="W10" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X10" s="22"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="21">
         <v>3</v>
       </c>
       <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="21" t="s">
+        <v>289</v>
+      </c>
       <c r="H11" s="16"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L11" s="25"/>
       <c r="N11" s="21"/>
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
       <c r="Q11" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R11" s="21"/>
       <c r="T11" s="21"/>
       <c r="U11" s="21"/>
       <c r="V11" s="21"/>
       <c r="W11" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="X11" s="21"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="C12" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="22">
         <v>3</v>
       </c>
       <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="F12" s="22" t="s">
+        <v>289</v>
+      </c>
       <c r="H12" s="23"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L12" s="26"/>
       <c r="N12" s="22"/>
       <c r="O12" s="22"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R12" s="22"/>
       <c r="T12" s="22"/>
       <c r="U12" s="22"/>
       <c r="V12" s="22"/>
       <c r="W12" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="X12" s="22"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
       <c r="C13" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="21">
         <v>1</v>
@@ -2493,28 +2535,28 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L13" s="25"/>
       <c r="N13" s="21"/>
       <c r="O13" s="21"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R13" s="21"/>
       <c r="T13" s="21"/>
       <c r="U13" s="21"/>
       <c r="V13" s="21"/>
       <c r="W13" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="X13" s="21"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B14" s="22"/>
       <c r="C14" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="22">
         <v>1</v>
@@ -2525,32 +2567,32 @@
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L14" s="26"/>
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R14" s="22"/>
       <c r="T14" s="22"/>
       <c r="U14" s="22"/>
       <c r="V14" s="22"/>
       <c r="W14" s="22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="X14" s="22"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="17">
         <f>SUM(D3:D14)</f>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -2558,27 +2600,27 @@
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L15" s="25"/>
       <c r="N15" s="21"/>
       <c r="O15" s="21"/>
       <c r="P15" s="21"/>
       <c r="Q15" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R15" s="21"/>
       <c r="T15" s="21"/>
       <c r="U15" s="21"/>
       <c r="V15" s="21"/>
       <c r="W15" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="X15" s="21"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>30</v>
@@ -2588,34 +2630,34 @@
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L16" s="26"/>
       <c r="N16" s="22"/>
       <c r="O16" s="22"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R16" s="22"/>
       <c r="T16" s="22"/>
       <c r="U16" s="22"/>
       <c r="V16" s="22"/>
       <c r="W16" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="X16" s="22"/>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="21">
         <v>1</v>
@@ -2626,28 +2668,28 @@
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L17" s="25"/>
       <c r="N17" s="21"/>
       <c r="O17" s="21"/>
       <c r="P17" s="21"/>
       <c r="Q17" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R17" s="21"/>
       <c r="T17" s="21"/>
       <c r="U17" s="21"/>
       <c r="V17" s="21"/>
       <c r="W17" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="X17" s="21"/>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" s="22"/>
       <c r="C18" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="22">
         <v>1</v>
@@ -2658,28 +2700,28 @@
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L18" s="26"/>
       <c r="N18" s="22"/>
       <c r="O18" s="22"/>
       <c r="P18" s="22"/>
       <c r="Q18" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R18" s="22"/>
       <c r="T18" s="22"/>
       <c r="U18" s="22"/>
       <c r="V18" s="22"/>
       <c r="W18" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X18" s="22"/>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="21">
         <v>1</v>
@@ -2690,28 +2732,28 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L19" s="25"/>
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R19" s="21"/>
       <c r="T19" s="21"/>
       <c r="U19" s="21"/>
       <c r="V19" s="21"/>
       <c r="W19" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="X19" s="21"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20" s="22"/>
       <c r="C20" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D20" s="22">
         <v>1</v>
@@ -2722,96 +2764,96 @@
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L20" s="26"/>
       <c r="N20" s="22"/>
       <c r="O20" s="22"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R20" s="22"/>
       <c r="T20" s="22"/>
       <c r="U20" s="22"/>
       <c r="V20" s="22"/>
       <c r="W20" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X20" s="22"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B21" s="21"/>
       <c r="C21" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" s="21">
         <v>1</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L21" s="25"/>
       <c r="N21" s="21"/>
       <c r="O21" s="21"/>
       <c r="P21" s="21"/>
       <c r="Q21" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R21" s="21"/>
       <c r="T21" s="21"/>
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
       <c r="W21" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X21" s="21"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
       <c r="C22" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="22">
         <v>1</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H22" s="23"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L22" s="26"/>
       <c r="N22" s="22"/>
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
       <c r="Q22" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R22" s="22"/>
       <c r="T22" s="22"/>
       <c r="U22" s="22"/>
       <c r="V22" s="22"/>
       <c r="W22" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X22" s="22"/>
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B23" s="21"/>
       <c r="C23" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="21">
         <v>1</v>
@@ -2822,28 +2864,28 @@
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L23" s="25"/>
       <c r="N23" s="21"/>
       <c r="O23" s="21"/>
       <c r="P23" s="21"/>
       <c r="Q23" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R23" s="21"/>
       <c r="T23" s="21"/>
       <c r="U23" s="21"/>
       <c r="V23" s="21"/>
       <c r="W23" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="X23" s="21"/>
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B24" s="22"/>
       <c r="C24" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="22">
         <v>1</v>
@@ -2854,28 +2896,28 @@
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L24" s="26"/>
       <c r="N24" s="22"/>
       <c r="O24" s="22"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R24" s="22"/>
       <c r="T24" s="22"/>
       <c r="U24" s="22"/>
       <c r="V24" s="22"/>
       <c r="W24" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X24" s="22"/>
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" s="21">
         <v>3</v>
@@ -2886,28 +2928,28 @@
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L25" s="25"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
       <c r="Q25" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R25" s="21"/>
       <c r="T25" s="21"/>
       <c r="U25" s="21"/>
       <c r="V25" s="21"/>
       <c r="W25" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="X25" s="21"/>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B26" s="22"/>
       <c r="C26" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" s="22">
         <v>3</v>
@@ -2918,28 +2960,28 @@
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L26" s="26"/>
       <c r="N26" s="22"/>
       <c r="O26" s="22"/>
       <c r="P26" s="22"/>
       <c r="Q26" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R26" s="22"/>
       <c r="T26" s="22"/>
       <c r="U26" s="22"/>
       <c r="V26" s="22"/>
       <c r="W26" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="X26" s="22"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
       <c r="C27" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" s="21">
         <v>1</v>
@@ -2950,27 +2992,27 @@
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L27" s="25"/>
       <c r="N27" s="21"/>
       <c r="O27" s="21"/>
       <c r="P27" s="21"/>
       <c r="Q27" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R27" s="21"/>
       <c r="T27" s="21"/>
       <c r="U27" s="21"/>
       <c r="V27" s="21"/>
       <c r="W27" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="X27" s="21"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="32">
@@ -2983,30 +3025,30 @@
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L28" s="26"/>
       <c r="N28" s="22"/>
       <c r="O28" s="22"/>
       <c r="P28" s="22"/>
       <c r="Q28" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R28" s="22"/>
       <c r="T28" s="22"/>
       <c r="U28" s="22"/>
       <c r="V28" s="22"/>
       <c r="W28" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="X28" s="22"/>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D29" s="21">
         <v>6</v>
@@ -3017,28 +3059,28 @@
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L29" s="25"/>
       <c r="N29" s="21"/>
       <c r="O29" s="21"/>
       <c r="P29" s="21"/>
       <c r="Q29" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R29" s="21"/>
       <c r="T29" s="21"/>
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
       <c r="W29" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X29" s="21"/>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B30" s="22"/>
       <c r="C30" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D30" s="22">
         <v>6</v>
@@ -3049,60 +3091,62 @@
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
       <c r="K30" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L30" s="26"/>
       <c r="N30" s="22"/>
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R30" s="22"/>
       <c r="T30" s="22"/>
       <c r="U30" s="22"/>
       <c r="V30" s="22"/>
       <c r="W30" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="X30" s="22"/>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B31" s="21"/>
       <c r="C31" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D31" s="21">
         <v>6</v>
       </c>
       <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
+      <c r="F31" s="21" t="s">
+        <v>292</v>
+      </c>
       <c r="H31" s="16"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L31" s="25"/>
       <c r="N31" s="21"/>
       <c r="O31" s="21"/>
       <c r="P31" s="21"/>
       <c r="Q31" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R31" s="21"/>
       <c r="T31" s="21"/>
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
       <c r="W31" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X31" s="21"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B32" s="22"/>
       <c r="C32" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D32" s="22">
         <v>6</v>
@@ -3113,28 +3157,28 @@
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L32" s="26"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
       <c r="P32" s="22"/>
       <c r="Q32" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R32" s="22"/>
       <c r="T32" s="22"/>
       <c r="U32" s="22"/>
       <c r="V32" s="22"/>
       <c r="W32" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="X32" s="22"/>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" s="21"/>
       <c r="C33" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D33" s="21">
         <v>1</v>
@@ -3145,28 +3189,28 @@
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L33" s="25"/>
       <c r="N33" s="21"/>
       <c r="O33" s="21"/>
       <c r="P33" s="21"/>
       <c r="Q33" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R33" s="21"/>
       <c r="T33" s="21"/>
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
       <c r="W33" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="X33" s="21"/>
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B34" s="22"/>
       <c r="C34" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D34" s="22">
         <v>1</v>
@@ -3177,28 +3221,28 @@
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
       <c r="K34" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L34" s="26"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
       <c r="P34" s="22"/>
       <c r="Q34" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R34" s="22"/>
       <c r="T34" s="22"/>
       <c r="U34" s="22"/>
       <c r="V34" s="22"/>
       <c r="W34" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="X34" s="22"/>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B35" s="21"/>
       <c r="C35" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D35" s="21">
         <v>1</v>
@@ -3209,28 +3253,28 @@
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L35" s="25"/>
       <c r="N35" s="21"/>
       <c r="O35" s="21"/>
       <c r="P35" s="21"/>
       <c r="Q35" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R35" s="21"/>
       <c r="T35" s="21"/>
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
       <c r="W35" s="21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="X35" s="21"/>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B36" s="22"/>
       <c r="C36" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D36" s="22">
         <v>1</v>
@@ -3241,28 +3285,28 @@
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
       <c r="K36" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L36" s="26"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
       <c r="P36" s="22"/>
       <c r="Q36" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R36" s="22"/>
       <c r="T36" s="22"/>
       <c r="U36" s="22"/>
       <c r="V36" s="22"/>
       <c r="W36" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X36" s="22"/>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" s="21"/>
       <c r="C37" s="21" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="D37" s="21">
         <v>1</v>
@@ -3272,120 +3316,114 @@
       <c r="H37" s="16"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
-      <c r="K37" s="12" t="s">
-        <v>136</v>
-      </c>
+      <c r="K37" s="12"/>
       <c r="L37" s="25"/>
-      <c r="N37" s="21"/>
-      <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="R37" s="21"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="21"/>
-      <c r="V37" s="21"/>
-      <c r="W37" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="X37" s="21"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="22"/>
+      <c r="X37" s="22"/>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B38" s="22"/>
       <c r="C38" s="22" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D38" s="22">
         <v>1</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="L38" s="26"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="R38" s="22"/>
-      <c r="T38" s="22"/>
-      <c r="U38" s="22"/>
-      <c r="V38" s="22"/>
-      <c r="W38" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="X38" s="22"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="L38" s="25"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="R38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="X38" s="21"/>
     </row>
     <row r="39" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B39" s="21"/>
       <c r="C39" s="21" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D39" s="21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="L39" s="25"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="R39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-      <c r="V39" s="21"/>
-      <c r="W39" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="X39" s="21"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L39" s="26"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="R39" s="22"/>
+      <c r="T39" s="22"/>
+      <c r="U39" s="22"/>
+      <c r="V39" s="22"/>
+      <c r="W39" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="X39" s="22"/>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B40" s="22"/>
       <c r="C40" s="22" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D40" s="22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="L40" s="26"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="R40" s="22"/>
-      <c r="T40" s="22"/>
-      <c r="U40" s="22"/>
-      <c r="V40" s="22"/>
-      <c r="W40" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="X40" s="22"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="L40" s="25"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="R40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="21"/>
+      <c r="W40" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="X40" s="21"/>
     </row>
     <row r="41" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B41" s="21"/>
@@ -3393,355 +3431,362 @@
         <v>279</v>
       </c>
       <c r="D41" s="21">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E41" s="21"/>
       <c r="F41" s="21"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="L41" s="25"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="R41" s="21"/>
-      <c r="T41" s="21"/>
-      <c r="U41" s="21"/>
-      <c r="V41" s="21"/>
-      <c r="W41" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="X41" s="21"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="L41" s="26"/>
+      <c r="N41" s="22"/>
+      <c r="O41" s="22"/>
+      <c r="P41" s="22"/>
+      <c r="Q41" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="R41" s="22"/>
+      <c r="T41" s="22"/>
+      <c r="U41" s="22"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="X41" s="22"/>
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B42" s="22"/>
       <c r="C42" s="22" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D42" s="22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="L42" s="26"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="R42" s="22"/>
-      <c r="T42" s="22"/>
-      <c r="U42" s="22"/>
-      <c r="V42" s="22"/>
-      <c r="W42" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="X42" s="22"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L42" s="25"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="R42" s="21"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="X42" s="21"/>
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B43" s="21"/>
       <c r="C43" s="21" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D43" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E43" s="21"/>
       <c r="F43" s="21"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="L43" s="25"/>
-      <c r="N43" s="21"/>
-      <c r="O43" s="21"/>
-      <c r="P43" s="21"/>
-      <c r="Q43" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="R43" s="21"/>
-      <c r="T43" s="21"/>
-      <c r="U43" s="21"/>
-      <c r="V43" s="21"/>
-      <c r="W43" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="X43" s="21"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="L43" s="26"/>
+      <c r="N43" s="22"/>
+      <c r="O43" s="22"/>
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="R43" s="22"/>
+      <c r="T43" s="22"/>
+      <c r="U43" s="22"/>
+      <c r="V43" s="22"/>
+      <c r="W43" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="X43" s="22"/>
     </row>
     <row r="44" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
+      <c r="C44" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="D44" s="22">
+        <v>5</v>
+      </c>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="L44" s="26"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="R44" s="22"/>
-      <c r="T44" s="22"/>
-      <c r="U44" s="22"/>
-      <c r="V44" s="22"/>
-      <c r="W44" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="X44" s="22"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="L44" s="25"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="21"/>
+      <c r="Q44" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="R44" s="21"/>
+      <c r="T44" s="21"/>
+      <c r="U44" s="21"/>
+      <c r="V44" s="21"/>
+      <c r="W44" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="X44" s="21"/>
     </row>
     <row r="45" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33">
+        <f>SUM(D29:D44)</f>
+        <v>54</v>
+      </c>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="L45" s="26"/>
+      <c r="N45" s="22"/>
+      <c r="O45" s="22"/>
+      <c r="P45" s="22"/>
+      <c r="Q45" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="R45" s="22"/>
+      <c r="T45" s="22"/>
+      <c r="U45" s="22"/>
+      <c r="V45" s="22"/>
+      <c r="W45" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="X45" s="22"/>
+    </row>
+    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B46" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="C46" s="22" t="s">
         <v>267</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D45" s="21">
-        <v>1</v>
-      </c>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="L45" s="25"/>
-      <c r="N45" s="21"/>
-      <c r="O45" s="21"/>
-      <c r="P45" s="21"/>
-      <c r="Q45" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="R45" s="21"/>
-      <c r="T45" s="21"/>
-      <c r="U45" s="21"/>
-      <c r="V45" s="21"/>
-      <c r="W45" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="X45" s="21"/>
-    </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B46" s="22"/>
-      <c r="C46" s="22" t="s">
-        <v>269</v>
       </c>
       <c r="D46" s="22">
         <v>1</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="L46" s="26"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="R46" s="22"/>
-      <c r="T46" s="22"/>
-      <c r="U46" s="22"/>
-      <c r="V46" s="22"/>
-      <c r="W46" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="X46" s="22"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="L46" s="25"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="R46" s="21"/>
+      <c r="T46" s="21"/>
+      <c r="U46" s="21"/>
+      <c r="V46" s="21"/>
+      <c r="W46" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="X46" s="21"/>
     </row>
     <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B47" s="21"/>
       <c r="C47" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D47" s="21">
         <v>1</v>
       </c>
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="L47" s="25"/>
-      <c r="N47" s="21"/>
-      <c r="O47" s="21"/>
-      <c r="P47" s="21"/>
-      <c r="Q47" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="R47" s="21"/>
-      <c r="T47" s="21"/>
-      <c r="U47" s="21"/>
-      <c r="V47" s="21"/>
-      <c r="W47" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="X47" s="21"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="L47" s="26"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="22"/>
+      <c r="P47" s="22"/>
+      <c r="Q47" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="R47" s="22"/>
+      <c r="T47" s="22"/>
+      <c r="U47" s="22"/>
+      <c r="V47" s="22"/>
+      <c r="W47" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="X47" s="22"/>
     </row>
     <row r="48" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B48" s="22"/>
       <c r="C48" s="22" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D48" s="22">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="L48" s="26"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="R48" s="22"/>
-      <c r="T48" s="22"/>
-      <c r="U48" s="22"/>
-      <c r="V48" s="22"/>
-      <c r="W48" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="X48" s="22"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="L48" s="25"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="21"/>
+      <c r="P48" s="21"/>
+      <c r="Q48" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="R48" s="21"/>
+      <c r="T48" s="21"/>
+      <c r="U48" s="21"/>
+      <c r="V48" s="21"/>
+      <c r="W48" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="X48" s="21"/>
     </row>
     <row r="49" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B49" s="21"/>
       <c r="C49" s="21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D49" s="21">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E49" s="21"/>
       <c r="F49" s="21"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="L49" s="25"/>
-      <c r="N49" s="21"/>
-      <c r="O49" s="21"/>
-      <c r="P49" s="21"/>
-      <c r="Q49" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="R49" s="21"/>
-      <c r="T49" s="21"/>
-      <c r="U49" s="21"/>
-      <c r="V49" s="21"/>
-      <c r="W49" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="X49" s="21"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="L49" s="26"/>
+      <c r="N49" s="22"/>
+      <c r="O49" s="22"/>
+      <c r="P49" s="22"/>
+      <c r="Q49" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="R49" s="22"/>
+      <c r="T49" s="22"/>
+      <c r="U49" s="22"/>
+      <c r="V49" s="22"/>
+      <c r="W49" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="X49" s="22"/>
     </row>
     <row r="50" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B50" s="22"/>
       <c r="C50" s="22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D50" s="22">
         <v>1</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="L50" s="26"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="22"/>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="R50" s="22"/>
-      <c r="T50" s="22"/>
-      <c r="U50" s="22"/>
-      <c r="V50" s="22"/>
-      <c r="W50" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="X50" s="22"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="L50" s="25"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
+      <c r="P50" s="21"/>
+      <c r="Q50" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="R50" s="21"/>
+      <c r="T50" s="21"/>
+      <c r="U50" s="21"/>
+      <c r="V50" s="21"/>
+      <c r="W50" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="X50" s="21"/>
     </row>
     <row r="51" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B51" s="21"/>
       <c r="C51" s="21" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D51" s="21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E51" s="21"/>
       <c r="F51" s="21"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="N51" s="21"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="R51" s="21"/>
-      <c r="T51" s="21"/>
-      <c r="U51" s="21"/>
-      <c r="V51" s="21"/>
-      <c r="W51" s="21" t="s">
-        <v>252</v>
-      </c>
-      <c r="X51" s="21"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L51" s="26"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="22"/>
+      <c r="Q51" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="R51" s="22"/>
+      <c r="T51" s="22"/>
+      <c r="U51" s="22"/>
+      <c r="V51" s="22"/>
+      <c r="W51" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="X51" s="22"/>
     </row>
     <row r="52" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B52" s="22"/>
       <c r="C52" s="22" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D52" s="22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
@@ -3750,28 +3795,28 @@
       <c r="J52" s="18"/>
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
-      <c r="N52" s="22"/>
-      <c r="O52" s="22"/>
-      <c r="P52" s="22"/>
-      <c r="Q52" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="R52" s="22"/>
-      <c r="T52" s="22"/>
-      <c r="U52" s="22"/>
-      <c r="V52" s="22"/>
-      <c r="W52" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="X52" s="22"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="21"/>
+      <c r="P52" s="21"/>
+      <c r="Q52" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="R52" s="21"/>
+      <c r="T52" s="21"/>
+      <c r="U52" s="21"/>
+      <c r="V52" s="21"/>
+      <c r="W52" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="X52" s="21"/>
     </row>
     <row r="53" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B53" s="21"/>
       <c r="C53" s="21" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D53" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E53" s="21"/>
       <c r="F53" s="21"/>
@@ -3780,25 +3825,29 @@
       <c r="J53" s="18"/>
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
-      <c r="N53" s="21"/>
-      <c r="O53" s="21"/>
-      <c r="P53" s="21"/>
-      <c r="Q53" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="R53" s="21"/>
-      <c r="T53" s="21"/>
-      <c r="U53" s="21"/>
-      <c r="V53" s="21"/>
-      <c r="W53" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="X53" s="21"/>
+      <c r="N53" s="22"/>
+      <c r="O53" s="22"/>
+      <c r="P53" s="22"/>
+      <c r="Q53" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="R53" s="22"/>
+      <c r="T53" s="22"/>
+      <c r="U53" s="22"/>
+      <c r="V53" s="22"/>
+      <c r="W53" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="X53" s="22"/>
     </row>
     <row r="54" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B54" s="22"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
+      <c r="C54" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="D54" s="22">
+        <v>5</v>
+      </c>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
       <c r="H54" s="18"/>
@@ -3806,20 +3855,20 @@
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
-      <c r="N54" s="22"/>
-      <c r="O54" s="22"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="R54" s="22"/>
-      <c r="T54" s="22"/>
-      <c r="U54" s="22"/>
-      <c r="V54" s="22"/>
-      <c r="W54" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="X54" s="22"/>
+      <c r="N54" s="21"/>
+      <c r="O54" s="21"/>
+      <c r="P54" s="21"/>
+      <c r="Q54" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="R54" s="21"/>
+      <c r="T54" s="21"/>
+      <c r="U54" s="21"/>
+      <c r="V54" s="21"/>
+      <c r="W54" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="X54" s="21"/>
     </row>
     <row r="55" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B55" s="21"/>
@@ -3832,28 +3881,25 @@
       <c r="J55" s="18"/>
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
-      <c r="N55" s="21"/>
-      <c r="O55" s="21"/>
-      <c r="P55" s="21"/>
-      <c r="Q55" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="R55" s="21"/>
-      <c r="T55" s="21"/>
-      <c r="U55" s="21"/>
-      <c r="V55" s="21"/>
-      <c r="W55" s="21" t="s">
-        <v>256</v>
-      </c>
-      <c r="X55" s="21"/>
+      <c r="N55" s="22"/>
+      <c r="O55" s="22"/>
+      <c r="P55" s="22"/>
+      <c r="Q55" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="R55" s="22"/>
+      <c r="T55" s="22"/>
+      <c r="U55" s="22"/>
+      <c r="V55" s="22"/>
+      <c r="W55" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="X55" s="22"/>
     </row>
     <row r="56" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
-      <c r="D56" s="22">
-        <f>SUM(D45:D53)</f>
-        <v>26</v>
-      </c>
+      <c r="D56" s="22"/>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
       <c r="H56" s="18"/>
@@ -3861,25 +3907,28 @@
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
-      <c r="N56" s="22"/>
-      <c r="O56" s="22"/>
-      <c r="P56" s="22"/>
-      <c r="Q56" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="R56" s="22"/>
-      <c r="T56" s="22"/>
-      <c r="U56" s="22"/>
-      <c r="V56" s="22"/>
-      <c r="W56" s="22" t="s">
-        <v>257</v>
-      </c>
-      <c r="X56" s="22"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="21"/>
+      <c r="P56" s="21"/>
+      <c r="Q56" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="R56" s="21"/>
+      <c r="T56" s="21"/>
+      <c r="U56" s="21"/>
+      <c r="V56" s="21"/>
+      <c r="W56" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="X56" s="21"/>
     </row>
     <row r="57" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
+      <c r="D57" s="21">
+        <f>SUM(D46:D54)</f>
+        <v>26</v>
+      </c>
       <c r="E57" s="21"/>
       <c r="F57" s="21"/>
       <c r="H57" s="18"/>
@@ -3887,21 +3936,20 @@
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
-      <c r="N57" s="31"/>
-      <c r="O57" s="31"/>
-      <c r="P57" s="31"/>
-      <c r="Q57" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="R57" s="21"/>
-      <c r="S57" s="12"/>
-      <c r="T57" s="31"/>
-      <c r="U57" s="31"/>
-      <c r="V57" s="31"/>
-      <c r="W57" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="X57" s="31"/>
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
+      <c r="P57" s="22"/>
+      <c r="Q57" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="R57" s="22"/>
+      <c r="T57" s="22"/>
+      <c r="U57" s="22"/>
+      <c r="V57" s="22"/>
+      <c r="W57" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="X57" s="22"/>
     </row>
     <row r="58" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B58" s="22"/>
@@ -3909,12 +3957,26 @@
       <c r="D58" s="22"/>
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
-      <c r="Q58" s="19"/>
-      <c r="R58" s="19"/>
-      <c r="S58" s="18"/>
-      <c r="T58" s="18"/>
-      <c r="W58" s="18"/>
-      <c r="X58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="N58" s="31"/>
+      <c r="O58" s="31"/>
+      <c r="P58" s="31"/>
+      <c r="Q58" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="R58" s="21"/>
+      <c r="S58" s="12"/>
+      <c r="T58" s="31"/>
+      <c r="U58" s="31"/>
+      <c r="V58" s="31"/>
+      <c r="W58" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="X58" s="31"/>
     </row>
     <row r="59" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B59" s="21"/>
@@ -3922,8 +3984,21 @@
       <c r="D59" s="21"/>
       <c r="E59" s="21"/>
       <c r="F59" s="21"/>
+      <c r="Q59" s="19"/>
+      <c r="R59" s="19"/>
+      <c r="S59" s="18"/>
+      <c r="T59" s="18"/>
       <c r="W59" s="18"/>
       <c r="X59" s="18"/>
+    </row>
+    <row r="60" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
+      <c r="W60" s="18"/>
+      <c r="X60" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>